<commit_message>
JVM and Tomcat Server knowledge
JVM and Tomcat Server knowledge
</commit_message>
<xml_diff>
--- a/Definitions/3_Definitions.xlsx
+++ b/Definitions/3_Definitions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Topics" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="234">
   <si>
     <t>Lucene</t>
   </si>
@@ -709,10 +709,6 @@
     <t>The Interpreter</t>
   </si>
   <si>
-    <t>1.We want to bridge the gap between planform independent byte code and the machine code of CPU we want to run our java application
-2. Whilst compilers do this better the interpreters still matters</t>
-  </si>
-  <si>
     <t>Source of inefficiency in interpreter</t>
   </si>
   <si>
@@ -1776,6 +1772,85 @@
   </si>
   <si>
     <t>http://camel.apache.org/getting-started.html</t>
+  </si>
+  <si>
+    <t>1.We want to bridge the gap between platform independent byte code and the machine code of CPU we want to run our java application
+2. Whilst compilers do this better the interpreters still matters</t>
+  </si>
+  <si>
+    <t>Java 8: From PermGen to MetaSpace</t>
+  </si>
+  <si>
+    <t>What this discussion about?</t>
+  </si>
+  <si>
+    <t>This article will share the information that we found so far on the PermGen successor: Metaspace. We will also compare the runtime behavior of the HotSpot 1.7 vs. HotSpot 1.8 (b75) when executing a Java program “leaking” class metadata objects</t>
+  </si>
+  <si>
+    <t>Metaspace</t>
+  </si>
+  <si>
+    <t>The JDK 8 HotSpot JVM is now using native memory for the representation of class metadata and is called Metaspace; similar to the Oracle JRockit and IBM JVM's.
+The good news is that it means no more java.lang.OutOfMemoryError: PermGen space problems and no need for you to tune and monitor this memory space anymore…not so fast. While this change is invisible by default, we will show you next that you will still need to worry about the class metadata memory footprint. Please also keep in mind that this new feature does not magically eliminate class and classloader memory leaks. You will need to track down these problems using a different approach and by learning the new naming convention.</t>
+  </si>
+  <si>
+    <t>PermGen Space in JDK8</t>
+  </si>
+  <si>
+    <t>1. This memory space is completely removed.
+2. The PermSize and MaxPermSize JVM arguments are ignored and a warning is issued if present at start-up</t>
+  </si>
+  <si>
+    <t>Metaspace memory allocation model</t>
+  </si>
+  <si>
+    <t>Most allocations for the class metadata are now allocated out of native memory.
+The klasses that were used to describe class metadata have been removed.</t>
+  </si>
+  <si>
+    <t>Metaspace capacity`</t>
+  </si>
+  <si>
+    <t>By default class metadata allocation is limited by the amount of available native memory (capacity will of course depend if you use a 32-bit JVM vs. 64-bit along with OS virtual memory availability).
+A new flag is available (MaxMetaspaceSize), allowing you to limit the amount of native memory used for class metadata. If you don’t specify this flag, the Metaspace will dynamically re-size depending of the application demand at runtime.</t>
+  </si>
+  <si>
+    <t>Metaspace garbage collection</t>
+  </si>
+  <si>
+    <t>Garbage collection of the dead classes and classloaders is triggered once the class metadata usage reaches the “MaxMetaspaceSize”.
+Proper monitoring &amp; tuning of the Metaspace will obviously be required in order to limit the frequency or delay of such garbage collections. Excessive Metaspace garbage collections may be a symptom of classes, classloaders memory leak or inadequate sizing for your application</t>
+  </si>
+  <si>
+    <t>Java heap space impact</t>
+  </si>
+  <si>
+    <t>Some miscellaneous data has been moved to the Java heap space. This means you may observe an increase of the Java heap space following a future JDK 8 upgrade</t>
+  </si>
+  <si>
+    <t>Metaspace monitoring</t>
+  </si>
+  <si>
+    <t>Metaspace usage is available from the HotSpot 1.8 verbose GC log output.
+Jstat &amp; JVisualVM have not been updated at this point based on our testing with b75 and the old PermGen space references are still present.</t>
+  </si>
+  <si>
+    <t>PermGen_vs_Metaspace_runtime_comparison</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">refer </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>images/i_JVM/f_PermGen_vs_Metaspace_runtime_comparison.pdf</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1859,7 +1934,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1887,6 +1962,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0000FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1954,7 +2035,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2018,6 +2099,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2050,6 +2134,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2398,7 +2494,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2440,7 +2536,7 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="24" t="s">
         <v>93</v>
       </c>
       <c r="B5" t="s">
@@ -2448,19 +2544,19 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="23"/>
+      <c r="A6" s="24"/>
       <c r="B6" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="23"/>
+      <c r="A7" s="24"/>
       <c r="B7" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="24" t="s">
         <v>104</v>
       </c>
       <c r="B8" t="s">
@@ -2468,22 +2564,22 @@
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="23"/>
+      <c r="A9" s="24"/>
       <c r="B9" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>213</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -2522,16 +2618,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="25"/>
+      <c r="B2" s="26"/>
     </row>
     <row r="3" spans="1:2" ht="120">
       <c r="A3" t="s">
@@ -2643,16 +2739,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="25"/>
+      <c r="B2" s="26"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="5" t="s">
@@ -2663,10 +2759,10 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="27"/>
+      <c r="B4" s="28"/>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="5" t="s">
@@ -2677,10 +2773,10 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="B6" s="28"/>
+      <c r="B6" s="29"/>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="7" t="s">
@@ -2699,7 +2795,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" ht="30">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="30" t="s">
         <v>54</v>
       </c>
       <c r="B9" s="14" t="s">
@@ -2707,13 +2803,13 @@
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="29"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="6" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="30" t="s">
         <v>55</v>
       </c>
       <c r="B11" s="7" t="s">
@@ -2721,7 +2817,7 @@
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="29"/>
+      <c r="A12" s="30"/>
       <c r="B12" s="9" t="s">
         <v>57</v>
       </c>
@@ -2743,7 +2839,7 @@
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="30" t="s">
         <v>61</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -2751,7 +2847,7 @@
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="29"/>
+      <c r="A16" s="30"/>
       <c r="B16" s="6" t="s">
         <v>62</v>
       </c>
@@ -2773,7 +2869,7 @@
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="30" t="s">
         <v>50</v>
       </c>
       <c r="B19" s="8" t="s">
@@ -2781,7 +2877,7 @@
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="29"/>
+      <c r="A20" s="30"/>
       <c r="B20" s="9" t="s">
         <v>66</v>
       </c>
@@ -2795,10 +2891,10 @@
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="28" t="s">
+      <c r="A22" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="B22" s="28"/>
+      <c r="B22" s="29"/>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="5"/>
@@ -2829,7 +2925,7 @@
       <c r="B28" s="5"/>
     </row>
     <row r="29" spans="1:2" ht="45">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="28" t="s">
         <v>30</v>
       </c>
       <c r="B29" s="7" t="s">
@@ -2837,7 +2933,7 @@
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="27"/>
+      <c r="A30" s="28"/>
       <c r="B30" s="6" t="s">
         <v>31</v>
       </c>
@@ -2945,16 +3041,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="25"/>
+      <c r="B2" s="26"/>
     </row>
     <row r="3" spans="1:2" ht="30">
       <c r="A3" t="s">
@@ -3051,22 +3147,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="25"/>
+      <c r="B2" s="26"/>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="B16" s="25"/>
+      <c r="B16" s="26"/>
     </row>
     <row r="17" spans="1:2" ht="60">
       <c r="A17" s="11" t="s">
@@ -3092,11 +3188,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:B70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3106,16 +3202,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="31"/>
+      <c r="B1" s="32"/>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="25"/>
+      <c r="B2" s="26"/>
     </row>
     <row r="3" spans="1:2" ht="30">
       <c r="A3" s="15" t="s">
@@ -3142,23 +3238,23 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="75">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="31" t="s">
         <v>113</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="60">
-      <c r="A7" s="30"/>
+      <c r="A7" s="31"/>
       <c r="B7" s="16" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="45">
-      <c r="A8" s="30"/>
+      <c r="A8" s="31"/>
       <c r="B8" s="16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="60">
@@ -3170,17 +3266,17 @@
       </c>
     </row>
     <row r="10" spans="1:2" ht="120">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="31" t="s">
         <v>117</v>
       </c>
       <c r="B10" s="16" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="90">
+      <c r="A11" s="31"/>
+      <c r="B11" s="16" t="s">
         <v>195</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="90">
-      <c r="A11" s="30"/>
-      <c r="B11" s="16" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -3196,15 +3292,15 @@
         <v>120</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="60">
       <c r="A14" s="20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="75">
@@ -3212,7 +3308,7 @@
         <v>121</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -3244,7 +3340,7 @@
         <v>128</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -3284,7 +3380,7 @@
         <v>137</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="30">
@@ -3296,23 +3392,23 @@
       </c>
     </row>
     <row r="26" spans="1:2" ht="45">
-      <c r="A26" s="30" t="s">
+      <c r="A26" s="31" t="s">
         <v>141</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="30">
-      <c r="A27" s="30"/>
+      <c r="A27" s="31"/>
       <c r="B27" s="16" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="45">
-      <c r="A28" s="30"/>
+      <c r="A28" s="31"/>
       <c r="B28" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="45">
@@ -3336,7 +3432,7 @@
         <v>147</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="45">
@@ -3352,7 +3448,7 @@
         <v>150</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -3368,7 +3464,7 @@
         <v>153</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="45">
@@ -3392,145 +3488,145 @@
         <v>158</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>159</v>
+        <v>214</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="60">
       <c r="A39" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="B39" s="16" t="s">
         <v>160</v>
-      </c>
-      <c r="B39" s="16" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="60">
       <c r="A40" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="B40" s="16" t="s">
         <v>162</v>
-      </c>
-      <c r="B40" s="16" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="45">
       <c r="A41" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="90">
       <c r="A42" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="B42" s="16" t="s">
         <v>165</v>
-      </c>
-      <c r="B42" s="16" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="45">
       <c r="A43" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="30">
       <c r="A44" s="18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="32" t="s">
-        <v>167</v>
-      </c>
-      <c r="B46" s="33"/>
+      <c r="A46" s="33" t="s">
+        <v>166</v>
+      </c>
+      <c r="B46" s="34"/>
     </row>
     <row r="47" spans="1:2" ht="60">
       <c r="A47" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="B47" s="16" t="s">
         <v>168</v>
       </c>
-      <c r="B47" s="16" t="s">
+    </row>
+    <row r="48" spans="1:2" ht="75">
+      <c r="A48" s="30" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" ht="75">
-      <c r="A48" s="29" t="s">
+      <c r="B48" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="B48" s="16" t="s">
+    </row>
+    <row r="49" spans="1:2" ht="90">
+      <c r="A49" s="30"/>
+      <c r="B49" s="16" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="90">
-      <c r="A49" s="29"/>
-      <c r="B49" s="16" t="s">
+    <row r="50" spans="1:2" ht="60">
+      <c r="A50" s="30" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" ht="60">
-      <c r="A50" s="29" t="s">
+      <c r="B50" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="B50" s="16" t="s">
+    </row>
+    <row r="51" spans="1:2" ht="45">
+      <c r="A51" s="30"/>
+      <c r="B51" s="16" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="45">
-      <c r="A51" s="29"/>
-      <c r="B51" s="16" t="s">
+    <row r="52" spans="1:2" ht="45">
+      <c r="A52" s="30"/>
+      <c r="B52" s="16" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="45">
-      <c r="A52" s="29"/>
-      <c r="B52" s="16" t="s">
+    <row r="53" spans="1:2" ht="105">
+      <c r="A53" s="30"/>
+      <c r="B53" s="16" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="105">
-      <c r="A53" s="29"/>
-      <c r="B53" s="16" t="s">
+    <row r="54" spans="1:2" ht="30">
+      <c r="A54" s="31" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" ht="30">
-      <c r="A54" s="30" t="s">
+      <c r="B54" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="B54" s="16" t="s">
+    </row>
+    <row r="55" spans="1:2" ht="45">
+      <c r="A55" s="31"/>
+      <c r="B55" s="16" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="45">
-      <c r="A55" s="30"/>
-      <c r="B55" s="16" t="s">
+    <row r="56" spans="1:2" ht="180">
+      <c r="A56" s="31"/>
+      <c r="B56" s="16" t="s">
         <v>180</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="180">
-      <c r="A56" s="30"/>
-      <c r="B56" s="16" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="75">
       <c r="A57" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="B57" s="16" t="s">
         <v>182</v>
-      </c>
-      <c r="B57" s="16" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="90">
@@ -3544,19 +3640,98 @@
     <row r="59" spans="1:2" ht="180">
       <c r="A59" s="17"/>
       <c r="B59" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="B60" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="B60" s="19" t="s">
-        <v>186</v>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="35" t="s">
+        <v>215</v>
+      </c>
+      <c r="B61" s="36"/>
+    </row>
+    <row r="62" spans="1:2" ht="30">
+      <c r="A62" s="37" t="s">
+        <v>216</v>
+      </c>
+      <c r="B62" s="38" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="105">
+      <c r="A63" s="37" t="s">
+        <v>218</v>
+      </c>
+      <c r="B63" s="23" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="30">
+      <c r="A64" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="B64" s="23" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="30">
+      <c r="A65" s="37" t="s">
+        <v>222</v>
+      </c>
+      <c r="B65" s="23" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="60">
+      <c r="A66" s="37" t="s">
+        <v>224</v>
+      </c>
+      <c r="B66" s="23" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="60">
+      <c r="A67" s="37" t="s">
+        <v>226</v>
+      </c>
+      <c r="B67" s="23" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="30">
+      <c r="A68" s="37" t="s">
+        <v>228</v>
+      </c>
+      <c r="B68" s="23" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="45">
+      <c r="A69" s="37" t="s">
+        <v>230</v>
+      </c>
+      <c r="B69" s="23" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="B70" s="23" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="A61:B61"/>
     <mergeCell ref="A48:A49"/>
     <mergeCell ref="A50:A53"/>
     <mergeCell ref="A54:A56"/>
@@ -3597,23 +3772,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="31"/>
+      <c r="B1" s="32"/>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="24" t="s">
-        <v>211</v>
-      </c>
-      <c r="B2" s="25"/>
+      <c r="A2" s="25" t="s">
+        <v>210</v>
+      </c>
+      <c r="B2" s="26"/>
     </row>
     <row r="3" spans="1:2" ht="105">
       <c r="A3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -3632,9 +3807,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3644,14 +3819,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="24"/>
-      <c r="B2" s="25"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>